<commit_message>
add ruby script to update LOG210 lab1
</commit_message>
<xml_diff>
--- a/LOG121/LOG121-notes.xlsx
+++ b/LOG121/LOG121-notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossypro/sources/ets/github-classroom-scripts/log121/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DB8434A-2A88-BB4D-A8EA-E6BBD49FD2FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B885574D-8FFA-8F42-A0AE-BEDA174ADEE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940"/>
   </bookViews>
   <sheets>
     <sheet name="LOG121-notes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="67">
   <si>
     <t>AQ92220</t>
   </si>
@@ -160,6 +160,42 @@
     <t>75.0</t>
   </si>
   <si>
+    <t>C11-MP2</t>
+  </si>
+  <si>
+    <t>112.5</t>
+  </si>
+  <si>
+    <t>162.0</t>
+  </si>
+  <si>
+    <t>200.0</t>
+  </si>
+  <si>
+    <t>174.4</t>
+  </si>
+  <si>
+    <t>35.0</t>
+  </si>
+  <si>
+    <t>C12-MP3</t>
+  </si>
+  <si>
+    <t>95.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0</t>
+  </si>
+  <si>
+    <t>C13-MP4</t>
+  </si>
+  <si>
+    <t>100.0 0.0</t>
+  </si>
+  <si>
+    <t>95.0 0.0</t>
+  </si>
+  <si>
     <t>Lab02</t>
   </si>
   <si>
@@ -173,6 +209,18 @@
   </si>
   <si>
     <t>92.0</t>
+  </si>
+  <si>
+    <t>Lab03</t>
+  </si>
+  <si>
+    <t>100.8</t>
+  </si>
+  <si>
+    <t>103.5</t>
+  </si>
+  <si>
+    <t>106.5</t>
   </si>
 </sst>
 </file>
@@ -1013,11 +1061,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1881,7 +1927,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B79" t="s">
         <v>46</v>
@@ -1892,7 +1938,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B80" t="s">
         <v>46</v>
@@ -1903,7 +1949,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B81" t="s">
         <v>46</v>
@@ -1914,7 +1960,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B82" t="s">
         <v>46</v>
@@ -1925,112 +1971,1069 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B83" t="s">
         <v>46</v>
       </c>
       <c r="C83" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B84" t="s">
         <v>46</v>
       </c>
       <c r="C84" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B85" t="s">
         <v>46</v>
       </c>
       <c r="C85" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B86" t="s">
         <v>46</v>
       </c>
       <c r="C86" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B87" t="s">
         <v>46</v>
       </c>
       <c r="C87" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B88" t="s">
         <v>46</v>
       </c>
       <c r="C88" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B89" t="s">
         <v>46</v>
       </c>
       <c r="C89" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B90" t="s">
         <v>46</v>
       </c>
       <c r="C90" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B91" t="s">
         <v>46</v>
       </c>
       <c r="C91" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B92" t="s">
         <v>46</v>
       </c>
       <c r="C92" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>17</v>
+      </c>
+      <c r="B93" t="s">
+        <v>46</v>
+      </c>
+      <c r="C93" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94" t="s">
+        <v>46</v>
+      </c>
+      <c r="C94" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>9</v>
+      </c>
+      <c r="B95" t="s">
+        <v>46</v>
+      </c>
+      <c r="C95" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>4</v>
+      </c>
+      <c r="B96" t="s">
+        <v>46</v>
+      </c>
+      <c r="C96" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" t="s">
+        <v>46</v>
+      </c>
+      <c r="C97" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>3</v>
+      </c>
+      <c r="B98" t="s">
+        <v>46</v>
+      </c>
+      <c r="C98" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99" t="s">
+        <v>46</v>
+      </c>
+      <c r="C99" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>13</v>
+      </c>
+      <c r="B100" t="s">
+        <v>46</v>
+      </c>
+      <c r="C100" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>11</v>
+      </c>
+      <c r="B101" t="s">
+        <v>46</v>
+      </c>
+      <c r="C101" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>36</v>
+      </c>
+      <c r="B102" t="s">
+        <v>46</v>
+      </c>
+      <c r="C102" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>14</v>
+      </c>
+      <c r="B103" t="s">
+        <v>46</v>
+      </c>
+      <c r="C103" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" t="s">
+        <v>46</v>
+      </c>
+      <c r="C104" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>10</v>
+      </c>
+      <c r="B105" t="s">
+        <v>46</v>
+      </c>
+      <c r="C105" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>13</v>
+      </c>
+      <c r="B106" t="s">
+        <v>52</v>
+      </c>
+      <c r="C106" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>11</v>
+      </c>
+      <c r="B107" t="s">
+        <v>52</v>
+      </c>
+      <c r="C107" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>36</v>
+      </c>
+      <c r="B108" t="s">
+        <v>52</v>
+      </c>
+      <c r="C108" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" t="s">
+        <v>52</v>
+      </c>
+      <c r="C109" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110" t="s">
+        <v>52</v>
+      </c>
+      <c r="C110" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111" t="s">
+        <v>52</v>
+      </c>
+      <c r="C111" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>6</v>
+      </c>
+      <c r="B112" t="s">
+        <v>52</v>
+      </c>
+      <c r="C112" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>15</v>
+      </c>
+      <c r="B113" t="s">
+        <v>52</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>16</v>
+      </c>
+      <c r="B114" t="s">
+        <v>52</v>
+      </c>
+      <c r="C114" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>17</v>
+      </c>
+      <c r="B115" t="s">
+        <v>52</v>
+      </c>
+      <c r="C115" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>9</v>
+      </c>
+      <c r="B116" t="s">
+        <v>52</v>
+      </c>
+      <c r="C116" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>23</v>
+      </c>
+      <c r="B117" t="s">
+        <v>52</v>
+      </c>
+      <c r="C117" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>27</v>
+      </c>
+      <c r="B118" t="s">
+        <v>52</v>
+      </c>
+      <c r="C118" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>28</v>
+      </c>
+      <c r="B119" t="s">
+        <v>52</v>
+      </c>
+      <c r="C119" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>25</v>
+      </c>
+      <c r="B120" t="s">
+        <v>52</v>
+      </c>
+      <c r="C120" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>29</v>
+      </c>
+      <c r="B121" t="s">
+        <v>52</v>
+      </c>
+      <c r="C121" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>21</v>
+      </c>
+      <c r="B122" t="s">
+        <v>52</v>
+      </c>
+      <c r="C122" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>24</v>
+      </c>
+      <c r="B123" t="s">
+        <v>52</v>
+      </c>
+      <c r="C123" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>19</v>
+      </c>
+      <c r="B124" t="s">
+        <v>52</v>
+      </c>
+      <c r="C124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>18</v>
+      </c>
+      <c r="B125" t="s">
+        <v>52</v>
+      </c>
+      <c r="C125" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>20</v>
+      </c>
+      <c r="B126" t="s">
+        <v>52</v>
+      </c>
+      <c r="C126" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>30</v>
+      </c>
+      <c r="B127" t="s">
+        <v>52</v>
+      </c>
+      <c r="C127" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>41</v>
+      </c>
+      <c r="B128" t="s">
+        <v>52</v>
+      </c>
+      <c r="C128" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>21</v>
+      </c>
+      <c r="B129" t="s">
+        <v>55</v>
+      </c>
+      <c r="C129" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>24</v>
+      </c>
+      <c r="B130" t="s">
+        <v>55</v>
+      </c>
+      <c r="C130" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>19</v>
+      </c>
+      <c r="B131" t="s">
+        <v>55</v>
+      </c>
+      <c r="C131" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>18</v>
+      </c>
+      <c r="B132" t="s">
+        <v>55</v>
+      </c>
+      <c r="C132" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>20</v>
+      </c>
+      <c r="B133" t="s">
+        <v>55</v>
+      </c>
+      <c r="C133" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>27</v>
+      </c>
+      <c r="B134" t="s">
+        <v>55</v>
+      </c>
+      <c r="C134" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>28</v>
+      </c>
+      <c r="B135" t="s">
+        <v>55</v>
+      </c>
+      <c r="C135" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>23</v>
+      </c>
+      <c r="B136" t="s">
+        <v>55</v>
+      </c>
+      <c r="C136" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>29</v>
+      </c>
+      <c r="B137" t="s">
+        <v>55</v>
+      </c>
+      <c r="C137" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>25</v>
+      </c>
+      <c r="B138" t="s">
+        <v>55</v>
+      </c>
+      <c r="C138" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>13</v>
+      </c>
+      <c r="B139" t="s">
+        <v>55</v>
+      </c>
+      <c r="C139" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>11</v>
+      </c>
+      <c r="B140" t="s">
+        <v>55</v>
+      </c>
+      <c r="C140" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>0</v>
+      </c>
+      <c r="B141" t="s">
+        <v>55</v>
+      </c>
+      <c r="C141" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>36</v>
+      </c>
+      <c r="B142" t="s">
+        <v>55</v>
+      </c>
+      <c r="C142" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>3</v>
+      </c>
+      <c r="B143" t="s">
+        <v>55</v>
+      </c>
+      <c r="C143" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>14</v>
+      </c>
+      <c r="B144" t="s">
+        <v>55</v>
+      </c>
+      <c r="C144" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>4</v>
+      </c>
+      <c r="B145" t="s">
+        <v>55</v>
+      </c>
+      <c r="C145" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>5</v>
+      </c>
+      <c r="B146" t="s">
+        <v>55</v>
+      </c>
+      <c r="C146" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>15</v>
+      </c>
+      <c r="B147" t="s">
+        <v>55</v>
+      </c>
+      <c r="C147" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>17</v>
+      </c>
+      <c r="B148" t="s">
+        <v>55</v>
+      </c>
+      <c r="C148" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>16</v>
+      </c>
+      <c r="B149" t="s">
+        <v>55</v>
+      </c>
+      <c r="C149" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>8</v>
+      </c>
+      <c r="B150" t="s">
+        <v>55</v>
+      </c>
+      <c r="C150" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>6</v>
+      </c>
+      <c r="B151" t="s">
+        <v>55</v>
+      </c>
+      <c r="C151" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>21</v>
+      </c>
+      <c r="B152" t="s">
+        <v>58</v>
+      </c>
+      <c r="C152" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>24</v>
+      </c>
+      <c r="B153" t="s">
+        <v>58</v>
+      </c>
+      <c r="C153" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>19</v>
+      </c>
+      <c r="B154" t="s">
+        <v>58</v>
+      </c>
+      <c r="C154" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>18</v>
+      </c>
+      <c r="B155" t="s">
+        <v>58</v>
+      </c>
+      <c r="C155" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>20</v>
+      </c>
+      <c r="B156" t="s">
+        <v>58</v>
+      </c>
+      <c r="C156" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>41</v>
+      </c>
+      <c r="B157" t="s">
+        <v>58</v>
+      </c>
+      <c r="C157" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>33</v>
+      </c>
+      <c r="B158" t="s">
+        <v>58</v>
+      </c>
+      <c r="C158" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>29</v>
+      </c>
+      <c r="B159" t="s">
+        <v>58</v>
+      </c>
+      <c r="C159" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>23</v>
+      </c>
+      <c r="B160" t="s">
+        <v>58</v>
+      </c>
+      <c r="C160" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>25</v>
+      </c>
+      <c r="B161" t="s">
+        <v>58</v>
+      </c>
+      <c r="C161" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>30</v>
+      </c>
+      <c r="B162" t="s">
+        <v>58</v>
+      </c>
+      <c r="C162" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>27</v>
+      </c>
+      <c r="B163" t="s">
+        <v>58</v>
+      </c>
+      <c r="C163" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>32</v>
+      </c>
+      <c r="B164" t="s">
+        <v>58</v>
+      </c>
+      <c r="C164" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>28</v>
+      </c>
+      <c r="B165" t="s">
+        <v>58</v>
+      </c>
+      <c r="C165" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>30</v>
+      </c>
+      <c r="B166" t="s">
+        <v>63</v>
+      </c>
+      <c r="C166" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>33</v>
+      </c>
+      <c r="B167" t="s">
+        <v>63</v>
+      </c>
+      <c r="C167" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>32</v>
+      </c>
+      <c r="B168" t="s">
+        <v>63</v>
+      </c>
+      <c r="C168" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>41</v>
+      </c>
+      <c r="B169" t="s">
+        <v>63</v>
+      </c>
+      <c r="C169" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>23</v>
+      </c>
+      <c r="B170" t="s">
+        <v>63</v>
+      </c>
+      <c r="C170" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>27</v>
+      </c>
+      <c r="B171" t="s">
+        <v>63</v>
+      </c>
+      <c r="C171" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>28</v>
+      </c>
+      <c r="B172" t="s">
+        <v>63</v>
+      </c>
+      <c r="C172" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>25</v>
+      </c>
+      <c r="B173" t="s">
+        <v>63</v>
+      </c>
+      <c r="C173" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>29</v>
+      </c>
+      <c r="B174" t="s">
+        <v>63</v>
+      </c>
+      <c r="C174" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>21</v>
+      </c>
+      <c r="B175" t="s">
+        <v>63</v>
+      </c>
+      <c r="C175" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>24</v>
+      </c>
+      <c r="B176" t="s">
+        <v>63</v>
+      </c>
+      <c r="C176" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>19</v>
+      </c>
+      <c r="B177" t="s">
+        <v>63</v>
+      </c>
+      <c r="C177" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>18</v>
+      </c>
+      <c r="B178" t="s">
+        <v>63</v>
+      </c>
+      <c r="C178" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>20</v>
+      </c>
+      <c r="B179" t="s">
+        <v>63</v>
+      </c>
+      <c r="C179" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>